<commit_message>
added stateAlert and updated all
</commit_message>
<xml_diff>
--- a/Output/1988/Hawaii/Hawaii.xlsx
+++ b/Output/1988/Hawaii/Hawaii.xlsx
@@ -9,14 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="17040" xr2:uid="{1C140856-F414-EA44-AC07-42AA93789268}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28100" windowHeight="17040" xr2:uid="{2913F83A-2769-E642-95C5-7E27384B9F5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$Z$108</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="148">
+  <si>
+    <t>State</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,9 @@
     <t>Note</t>
   </si>
   <si>
+    <t>HI</t>
+  </si>
+  <si>
     <t>AHUIMANU</t>
   </si>
   <si>
@@ -116,6 +119,9 @@
     <t>ALIAMUNU GOVERNMENT RESERVE</t>
   </si>
   <si>
+    <t>ANAHOLA</t>
+  </si>
+  <si>
     <t>See KALAHEO, HI</t>
   </si>
   <si>
@@ -137,6 +143,9 @@
     <t>EWA</t>
   </si>
   <si>
+    <t>EWA BEACH</t>
+  </si>
+  <si>
     <t>FOSTER VILLAGE</t>
   </si>
   <si>
@@ -245,9 +254,6 @@
     <t>KAPAA</t>
   </si>
   <si>
-    <t>See KAUAI ISLAND (eastern portion), H|</t>
-  </si>
-  <si>
     <t>KAPAHULU</t>
   </si>
   <si>
@@ -275,18 +281,15 @@
     <t>KEAUHOU</t>
   </si>
   <si>
-    <t>See KAILUA KONA, HI.</t>
-  </si>
-  <si>
     <t>KEKAHA</t>
   </si>
   <si>
+    <t>KIHEI</t>
+  </si>
+  <si>
     <t>Kilanea Military Camp</t>
   </si>
   <si>
-    <t>See PAHALA, HI.</t>
-  </si>
-  <si>
     <t>KILAUEA</t>
   </si>
   <si>
@@ -353,6 +356,9 @@
     <t>MILILANI</t>
   </si>
   <si>
+    <t>MOANALUA</t>
+  </si>
+  <si>
     <t>MOILIIU</t>
   </si>
   <si>
@@ -389,9 +395,6 @@
     <t>PAHOA</t>
   </si>
   <si>
-    <t xml:space="preserve">See HILO, HI. </t>
-  </si>
-  <si>
     <t>PAUOA</t>
   </si>
   <si>
@@ -401,6 +404,9 @@
     <t>PEARL HARBOR GOVERNMENT RESERVE</t>
   </si>
   <si>
+    <t>PRINCEVILLE-HANALEI</t>
+  </si>
+  <si>
     <t>PUKALANI</t>
   </si>
   <si>
@@ -416,6 +422,9 @@
     <t>SUNSET BEACH</t>
   </si>
   <si>
+    <t>VOLCANO VILLAGE</t>
+  </si>
+  <si>
     <t>WAHIAWA</t>
   </si>
   <si>
@@ -440,6 +449,9 @@
     <t>WAILUA</t>
   </si>
   <si>
+    <t>WAILUA HOMESTEADS</t>
+  </si>
+  <si>
     <t>WAILUKU</t>
   </si>
   <si>
@@ -449,9 +461,6 @@
     <t>WAIMEA</t>
   </si>
   <si>
-    <t xml:space="preserve">See KALAHEO, HI. </t>
-  </si>
-  <si>
     <t>Waiohinu</t>
   </si>
   <si>
@@ -459,45 +468,6 @@
   </si>
   <si>
     <t>WAIPIO</t>
-  </si>
-  <si>
-    <t>KIHEI</t>
-  </si>
-  <si>
-    <t>MOANALUA</t>
-  </si>
-  <si>
-    <t>PRINCEVILLE-HANALEI</t>
-  </si>
-  <si>
-    <t>VOLCANO VILLAGE</t>
-  </si>
-  <si>
-    <t>WAILUA HOMESTEADS</t>
-  </si>
-  <si>
-    <t>ANAHOLA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Below 100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>See HONOLULU, HI.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EWA BEACH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>State</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -866,7 +836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D454EC-F993-924F-99A4-0202DCCFAED5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E2BC44-6E3D-1C4E-8672-920659C3282B}">
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -878,90 +848,90 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -976,37 +946,37 @@
         <v>10144</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K2" s="1">
         <v>6500</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -1027,21 +997,21 @@
         <v>26</v>
       </c>
       <c r="Y2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F3" s="2">
         <v>29861</v>
@@ -1053,34 +1023,34 @@
         <v>1541</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K3" s="1">
         <v>2161</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -1101,21 +1071,21 @@
         <v>6</v>
       </c>
       <c r="Y3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2">
         <v>27193</v>
@@ -1124,13 +1094,13 @@
         <v>12930</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K4">
         <v>551</v>
@@ -1151,10 +1121,10 @@
         <v>1476</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -1175,15 +1145,15 @@
         <v>9</v>
       </c>
       <c r="Y4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1198,37 +1168,37 @@
         <v>186777</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K5" s="1">
         <v>162500</v>
       </c>
       <c r="L5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -1240,7 +1210,7 @@
         <v>268300</v>
       </c>
       <c r="V5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="W5">
         <v>36</v>
@@ -1249,15 +1219,15 @@
         <v>6</v>
       </c>
       <c r="Y5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1275,10 +1245,10 @@
         <v>3757</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K6">
         <v>928</v>
@@ -1290,19 +1260,19 @@
         <v>2046</v>
       </c>
       <c r="N6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1323,15 +1293,15 @@
         <v>17</v>
       </c>
       <c r="Y6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1343,40 +1313,40 @@
         <v>30308</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -1385,27 +1355,27 @@
         <v>0</v>
       </c>
       <c r="U7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="V7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="X7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Y7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1420,37 +1390,37 @@
         <v>6443</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K8" s="1">
         <v>3800</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -1471,15 +1441,15 @@
         <v>16</v>
       </c>
       <c r="Y8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1494,37 +1464,37 @@
         <v>3837</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K9" s="1">
         <v>2361</v>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S9">
         <v>1</v>
@@ -1533,10 +1503,10 @@
         <v>0</v>
       </c>
       <c r="U9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="V9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="W9">
         <v>20</v>
@@ -1545,21 +1515,21 @@
         <v>15</v>
       </c>
       <c r="Y9" t="s">
-        <v>150</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2">
         <v>24987</v>
@@ -1568,13 +1538,13 @@
         <v>2400</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K10" s="1">
         <v>1800</v>
@@ -1586,19 +1556,19 @@
         <v>200</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S10">
         <v>1</v>
@@ -1607,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="V10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="W10">
         <v>35</v>
@@ -1619,15 +1589,15 @@
         <v>20</v>
       </c>
       <c r="Y10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1642,13 +1612,13 @@
         <v>14637</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K11">
         <v>544</v>
@@ -1666,13 +1636,13 @@
         <v>693</v>
       </c>
       <c r="P11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S11">
         <v>1</v>
@@ -1684,24 +1654,24 @@
         <v>24990</v>
       </c>
       <c r="V11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="W11">
         <v>34</v>
       </c>
       <c r="X11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Y11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1716,37 +1686,37 @@
         <v>953</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K12">
         <v>245</v>
       </c>
       <c r="L12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S12">
         <v>1</v>
@@ -1755,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="V12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="W12">
         <v>20</v>
@@ -1767,21 +1737,21 @@
         <v>11</v>
       </c>
       <c r="Y12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F13" s="2">
         <v>29526</v>
@@ -1790,37 +1760,37 @@
         <v>1156</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="Q13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -1841,1345 +1811,1344 @@
         <v>8</v>
       </c>
       <c r="Y13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
         <v>62</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B61" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B78" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B79" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B81" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B84" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B86" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B87" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B88" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B89" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B90" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B91" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B92" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B93" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B94" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B97" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B98" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B99" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B100" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B101" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B102" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B103" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>140</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B106" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B107" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B108" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:Z108">
+  <sortState ref="A2:Z110">
     <sortCondition ref="C1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>